<commit_message>
inclusion of 'experiments' sheet to describe a set of experiments to run
</commit_message>
<xml_diff>
--- a/xlsxPCES/template/template.xlsx
+++ b/xlsxPCES/template/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicol/Dropbox/gitTemp/pcesbld/xlsxPCES/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicol/Dropbox/github-repos/pcesbld/xlsxPCES/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEDE880-F2AD-794E-BB19-52B8EBE5C62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F32B9E-EFC5-D44E-B887-BED1EC037310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="820" windowWidth="24640" windowHeight="18040" activeTab="4" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
+    <workbookView xWindow="5880" yWindow="820" windowWidth="24640" windowHeight="18040" activeTab="5" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="topo" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="execTime" sheetId="4" r:id="rId3"/>
     <sheet name="mapping" sheetId="2" r:id="rId4"/>
     <sheet name="netParams" sheetId="5" r:id="rId5"/>
+    <sheet name="experiments" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="123">
   <si>
     <t>Networks</t>
   </si>
@@ -376,13 +377,43 @@
   </si>
   <si>
     <t>Wireless-Connections</t>
+  </si>
+  <si>
+    <t>Experiments</t>
+  </si>
+  <si>
+    <t>$crypto,cp</t>
+  </si>
+  <si>
+    <t>$bndwdth,netParams</t>
+  </si>
+  <si>
+    <t>AES-256-CBC</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>AES-128-CBC</t>
+  </si>
+  <si>
+    <t>#exp-1</t>
+  </si>
+  <si>
+    <t>#exp-2</t>
+  </si>
+  <si>
+    <t>#exp-3</t>
+  </si>
+  <si>
+    <t>#exp-4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -524,8 +555,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -744,6 +781,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB5E6A2"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -949,7 +992,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -960,6 +1003,11 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2059,7 +2107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04436424-07DF-B343-BAAE-706A3CFD4756}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -2255,4 +2303,90 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E5D7B3-B8B2-494B-8744-E4EF039717CC}">
+  <dimension ref="A2:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="12">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="12">
+        <v>10</v>
+      </c>
+      <c r="D7" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>